<commit_message>
create searched Attendance with all combination and create checkin and checkout
</commit_message>
<xml_diff>
--- a/wwwroot/Uploads/AttendanceTest.xlsx
+++ b/wwwroot/Uploads/AttendanceTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{387EBB5A-1223-461A-947C-40829006902B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE8643D-0C91-45AD-B2E2-613ABC4A55D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3C14AF9-3291-460A-ACE3-FEA6D911BA62}"/>
   </bookViews>
@@ -391,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C99FB1A-B472-4C8F-B68D-E1D9CC37FE0C}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41:D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,7 +428,7 @@
         <v>45181.493750000001</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -442,7 +442,7 @@
         <v>45182.493750000001</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -456,7 +456,7 @@
         <v>45183.493750000001</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>